<commit_message>
data for states al, ak, az, ca, ct, partial id
</commit_message>
<xml_diff>
--- a/data/resort_tracking.xlsx
+++ b/data/resort_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\backup\repo\one-stop-ski-trip\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACDA659-2F41-48D6-8641-78803B55E4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73D19DC-6739-4FDD-89ED-3EFB7CE94C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2121,9 +2121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P365"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2182,1429 +2180,1429 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>1800</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1650</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>150</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>2</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>2</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>10</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>0.5</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>5</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>0.5</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>5</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>0</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>33.4</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>-86.08</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>3939</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>250</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>2500</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>9</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>73</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>1500</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>0.11</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>165</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>0.52</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <v>780</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>0.37</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>555</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <v>60.97</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <v>-149.11000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>3900</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>2500</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1400</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>4</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>25</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>320</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>0.2</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>64</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>0.5</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <v>160</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>0.3</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>96</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="1">
         <v>61.24</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <v>-149.61000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>2600</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1200</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>1540</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>4</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>31</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>640</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>0.2</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>128</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>0.4</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <v>256</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <v>0.4</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <v>256</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <v>58.3</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <v>-134.55000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>894</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>600</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>294</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>10</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>30</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>0.8</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>24</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>0.1</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <v>3</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <v>0.1</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <v>3</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="1">
         <v>61.43</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <v>-149.44</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>1987</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>680</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>1307</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>14</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>35</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>200</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>0.15</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>30</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>0.65</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="1">
         <v>130</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="1">
         <v>0.2</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="1">
         <v>40</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="1">
         <v>64.92</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="1">
         <v>-147.94</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>1050</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>3</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>100</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>0.2</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>20</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>0.4</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="1">
         <v>40</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="1">
         <v>0.4</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="1">
         <v>40</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="1">
         <v>63.52</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="1">
         <v>-146.54</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>11500</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>9200</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>2300</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>6</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>40</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>777</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>0.37</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <v>287.49</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>0.42</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="1">
         <v>326.33999999999997</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="1">
         <v>0.21</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="1">
         <v>163.16999999999999</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="1">
         <v>35.327820000000003</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="1">
         <v>-111.69517</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>8150</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>7500</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>600</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>2</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>12</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>37</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>0.3</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <v>11.1</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="1">
         <v>0.5</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="1">
         <v>18.5</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="1">
         <v>0.2</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="1">
         <v>7.4</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="1">
         <v>35.1</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="1">
         <v>-112.23</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>9150</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>8200</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>950</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>3</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>21</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>200</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>0.2</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <v>40</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>0.38</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <v>76</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="1">
         <v>0.42</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="1">
         <v>84</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="1">
         <v>32.450000000000003</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="1">
         <v>-110.76</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>1100</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>9200</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>1800</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>8</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>65</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>800</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>0.4</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>320</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <v>0.4</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <v>320</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="1">
         <v>0.2</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="1">
         <v>160</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="1">
         <v>34.020000000000003</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="1">
         <v>-109.53</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>8673</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>6385</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>2288</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>13</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>100</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>2400</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>0.25</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>600</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <v>0.4</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="1">
         <v>960</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="1">
         <v>0.35</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="1">
         <v>840</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="1">
         <v>39.17</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="1">
         <v>-120.22</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>8805</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>7140</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>1665</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>12</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>748</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>0.3</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>224.4</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <v>0.4</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="1">
         <v>299.2</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="1">
         <v>0.3</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="1">
         <v>224.4</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="1">
         <v>37.1</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="1">
         <v>-119.1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>8500</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>6600</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>1900</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>9</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>75</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>1680</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <v>0.25</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <v>420</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="1">
         <v>0.4</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="1">
         <v>672</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="1">
         <v>0.35</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="1">
         <v>588</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="1">
         <v>39.200000000000003</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="1">
         <v>-122.44</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>7700</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>7200</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>500</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>6</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>41</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>480</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>0.3</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <v>144</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="1">
         <v>264</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="1">
         <v>0.15</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="1">
         <v>72</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="1">
         <v>39.33</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="1">
         <v>-120.35</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>8709</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>7030</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>1679</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>11</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>45</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>1200</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <v>0.11</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <v>132</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="1">
         <v>336</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="1">
         <v>0.61</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="1">
         <v>732</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="1">
         <v>40.9</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="1">
         <v>-123.34</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>8200</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>6600</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>1600</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>12</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>67</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>852</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <v>0.2</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <v>170.4</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="1">
         <v>0.4</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="1">
         <v>340.8</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="1">
         <v>0.4</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18" s="1">
         <v>340.8</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="1">
         <v>38.14</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="1">
         <v>-120.03</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>7781</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>7031</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>750</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>8</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>53</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="1">
         <v>503</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="1">
         <v>0.25</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <v>125.75</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1">
         <v>0.5</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="1">
         <v>251.5</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="1">
         <v>0.25</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="1">
         <v>125.75</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O19" s="1">
         <v>39.31</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P19" s="1">
         <v>-120.34</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>10067</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>6540</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>3527</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>29</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>97</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>4800</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <v>0.2</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
         <v>960</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>0.45</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="1">
         <v>2160</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="1">
         <v>0.35</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="1">
         <v>1680</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O20" s="1">
         <v>38.935299999999998</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P20" s="1">
         <v>-119.94</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>7800</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>6230</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>1570</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>8</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>64</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="1">
         <v>1260</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="1">
         <v>0.15</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="1">
         <v>189</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="1">
         <v>0.5</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="1">
         <v>630</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="1">
         <v>0.35</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21" s="1">
         <v>441</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O21" s="1">
         <v>39.08</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P21" s="1">
         <v>-120.17</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>9800</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>7800</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>2000</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>15</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>81</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="1">
         <v>2300</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="1">
         <v>0.15</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="1">
         <v>345</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>0.5</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="1">
         <v>1150</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="1">
         <v>0.35</v>
       </c>
-      <c r="N22" s="2">
+      <c r="N22" s="1">
         <v>805</v>
       </c>
-      <c r="O22" s="2">
+      <c r="O22" s="1">
         <v>38.683999999999997</v>
       </c>
-      <c r="P22" s="2">
+      <c r="P22" s="1">
         <v>-120.068</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>11053</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>7953</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>3100</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>28</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>150</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="1">
         <v>3500</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="1">
         <v>0.25</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="1">
         <v>875</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1">
         <v>0.4</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="1">
         <v>1400</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="1">
         <v>0.35</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23" s="1">
         <v>1225</v>
       </c>
-      <c r="O23" s="2">
+      <c r="O23" s="1">
         <v>41.73</v>
       </c>
-      <c r="P23" s="2">
+      <c r="P23" s="1">
         <v>-121.37</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>9700</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>7900</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>1800</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>6</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>43</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <v>1200</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="1">
         <v>0.2</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="1">
         <v>240</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="1">
         <v>0.3</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="1">
         <v>360</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="1">
         <v>0.5</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="1">
         <v>600</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O24" s="1">
         <v>39.340000000000003</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P24" s="1">
         <v>-119.92</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>8200</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>6600</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>1600</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>12</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>28</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
         <v>290</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <v>0.25</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="1">
         <v>72.5</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1">
         <v>0.4</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="1">
         <v>116</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="1">
         <v>0.35</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="1">
         <v>101.5</v>
       </c>
-      <c r="O25" s="2">
+      <c r="O25" s="1">
         <v>41.96</v>
       </c>
-      <c r="P25" s="2">
+      <c r="P25" s="1">
         <v>-122.44</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="1">
         <v>5</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>32</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="1">
         <v>425</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="1">
         <v>0.2</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="1">
         <v>85</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="1">
         <v>233.75</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="1">
         <v>0.25</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="1">
         <v>106.25</v>
       </c>
-      <c r="O26" s="2">
+      <c r="O26" s="1">
         <v>41.31</v>
       </c>
-      <c r="P26" s="2">
+      <c r="P26" s="1">
         <v>-122.29</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>8610</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>6800</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>1810</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="1">
         <v>20</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
         <v>17</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="1">
         <v>3170</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="1">
         <v>0.13</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="1">
         <v>412.1</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="1">
         <v>0.6</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="1">
         <v>1902</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="1">
         <v>0.27</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N27" s="1">
         <v>855.9</v>
       </c>
-      <c r="O27" s="2">
+      <c r="O27" s="1">
         <v>38.58</v>
       </c>
-      <c r="P27" s="2">
+      <c r="P27" s="1">
         <v>-121.75</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>8852</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>6640</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>2212</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="1">
         <v>14</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>46</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="1">
         <v>2000</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="1">
         <v>0.25</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="1">
         <v>500</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="1">
         <v>0.5</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="1">
         <v>1000</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="1">
         <v>0.25</v>
       </c>
-      <c r="N28" s="2">
+      <c r="N28" s="1">
         <v>500</v>
       </c>
-      <c r="O28" s="2">
+      <c r="O28" s="1">
         <v>38.81</v>
       </c>
-      <c r="P28" s="2">
+      <c r="P28" s="1">
         <v>-120.07</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>9050</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>6200</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>2850</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="1">
         <v>30</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>170</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="1">
         <v>3600</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="1">
         <v>0.25</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="1">
         <v>900</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="1">
         <v>0.45</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="1">
         <v>1620</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="1">
         <v>0.3</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N29" s="1">
         <v>1080</v>
       </c>
-      <c r="O29" s="2">
+      <c r="O29" s="1">
         <v>36.74</v>
       </c>
-      <c r="P29" s="2">
+      <c r="P29" s="1">
         <v>-119.25</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>8383</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>6883</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>1500</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>13</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>103</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="1">
         <v>1650</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="1">
         <v>0.17</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="1">
         <v>280.5</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="1">
         <v>0.45</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="1">
         <v>742.5</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="1">
         <v>0.38</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N30" s="1">
         <v>627</v>
       </c>
-      <c r="O30" s="2">
+      <c r="O30" s="1">
         <v>39.270000000000003</v>
       </c>
-      <c r="P30" s="2">
+      <c r="P30" s="1">
         <v>-120.3</v>
       </c>
     </row>
@@ -4808,747 +4806,747 @@
         <v>-106.6</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>1600</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="1">
         <v>960</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55" s="1">
         <v>650</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55" s="1">
         <v>7</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55" s="1">
         <v>25</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55" s="1">
         <v>107</v>
       </c>
-      <c r="I55" s="2">
+      <c r="I55" s="1">
         <v>0.2</v>
       </c>
-      <c r="J55" s="2">
+      <c r="J55" s="1">
         <v>21.4</v>
       </c>
-      <c r="K55" s="2">
+      <c r="K55" s="1">
         <v>0.6</v>
       </c>
-      <c r="L55" s="2">
+      <c r="L55" s="1">
         <v>64.2</v>
       </c>
-      <c r="M55" s="2">
+      <c r="M55" s="1">
         <v>0.2</v>
       </c>
-      <c r="N55" s="2">
+      <c r="N55" s="1">
         <v>21.4</v>
       </c>
-      <c r="O55" s="2">
+      <c r="O55" s="1">
         <v>41.83</v>
       </c>
-      <c r="P55" s="2">
+      <c r="P55" s="1">
         <v>-73.31</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>525</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="1">
         <v>100</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="1">
         <v>425</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F56" s="1">
         <v>7</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56" s="1">
         <v>14</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H56" s="1">
         <v>51</v>
       </c>
-      <c r="I56" s="2">
+      <c r="I56" s="1">
         <v>0.33</v>
       </c>
-      <c r="J56" s="2">
+      <c r="J56" s="1">
         <v>16.829999999999998</v>
       </c>
-      <c r="K56" s="2">
+      <c r="K56" s="1">
         <v>0.42</v>
       </c>
-      <c r="L56" s="2">
+      <c r="L56" s="1">
         <v>21.42</v>
       </c>
-      <c r="M56" s="2">
+      <c r="M56" s="1">
         <v>0.25</v>
       </c>
-      <c r="N56" s="2">
+      <c r="N56" s="1">
         <v>12.75</v>
       </c>
-      <c r="O56" s="2">
+      <c r="O56" s="1">
         <v>41.61</v>
       </c>
-      <c r="P56" s="2">
+      <c r="P56" s="1">
         <v>-72.94</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+    <row r="57" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="1">
         <v>1075</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="1">
         <v>450</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="1">
         <v>625</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57" s="1">
         <v>5</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G57" s="1">
         <v>15</v>
       </c>
-      <c r="H57" s="2">
+      <c r="H57" s="1">
         <v>65</v>
       </c>
-      <c r="I57" s="2">
+      <c r="I57" s="1">
         <v>0.5</v>
       </c>
-      <c r="J57" s="2">
+      <c r="J57" s="1">
         <v>32.5</v>
       </c>
-      <c r="K57" s="2">
+      <c r="K57" s="1">
         <v>0.25</v>
       </c>
-      <c r="L57" s="2">
+      <c r="L57" s="1">
         <v>16.25</v>
       </c>
-      <c r="M57" s="2">
+      <c r="M57" s="1">
         <v>0.25</v>
       </c>
-      <c r="N57" s="2">
+      <c r="N57" s="1">
         <v>16.25</v>
       </c>
-      <c r="O57" s="2">
+      <c r="O57" s="1">
         <v>41.6</v>
       </c>
-      <c r="P57" s="2">
+      <c r="P57" s="1">
         <v>-73.09</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>850</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="1">
         <v>550</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="1">
         <v>300</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F58" s="1">
         <v>6</v>
       </c>
-      <c r="G58" s="2">
+      <c r="G58" s="1">
         <v>15</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H58" s="1">
         <v>100</v>
       </c>
-      <c r="I58" s="2">
+      <c r="I58" s="1">
         <v>0.33</v>
       </c>
-      <c r="J58" s="2">
+      <c r="J58" s="1">
         <v>33</v>
       </c>
-      <c r="K58" s="2">
+      <c r="K58" s="1">
         <v>0.34</v>
       </c>
-      <c r="L58" s="2">
+      <c r="L58" s="1">
         <v>34</v>
       </c>
-      <c r="M58" s="2">
+      <c r="M58" s="1">
         <v>0.33</v>
       </c>
-      <c r="N58" s="2">
+      <c r="N58" s="1">
         <v>33</v>
       </c>
-      <c r="O58" s="2">
+      <c r="O58" s="1">
         <v>41.55</v>
       </c>
-      <c r="P58" s="2">
+      <c r="P58" s="1">
         <v>-73.22</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="1">
         <v>4800</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="1">
         <v>4000</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59" s="1">
         <v>684</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F59" s="1">
         <v>2</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H59" s="1">
         <v>140</v>
       </c>
-      <c r="I59" s="2">
+      <c r="I59" s="1">
         <v>0.25</v>
       </c>
-      <c r="J59" s="2">
+      <c r="J59" s="1">
         <v>35</v>
       </c>
-      <c r="K59" s="2">
+      <c r="K59" s="1">
         <v>0.4</v>
       </c>
-      <c r="L59" s="2">
+      <c r="L59" s="1">
         <v>56</v>
       </c>
-      <c r="M59" s="2">
+      <c r="M59" s="1">
         <v>0.35</v>
       </c>
-      <c r="N59" s="2">
+      <c r="N59" s="1">
         <v>49</v>
       </c>
-      <c r="O59" s="2">
+      <c r="O59" s="1">
         <v>44.37</v>
       </c>
-      <c r="P59" s="2">
+      <c r="P59" s="1">
         <v>-114.35</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+    <row r="60" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <v>7582</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="1">
         <v>5800</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="1">
         <v>1800</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F60" s="1">
         <v>8</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G60" s="1">
         <v>66</v>
       </c>
-      <c r="H60" s="2">
+      <c r="H60" s="1">
         <v>2600</v>
       </c>
-      <c r="I60" s="2">
+      <c r="I60" s="1">
         <v>0.22</v>
       </c>
-      <c r="J60" s="2">
+      <c r="J60" s="1">
         <v>572</v>
       </c>
-      <c r="K60" s="2">
+      <c r="K60" s="1">
         <v>0.45</v>
       </c>
-      <c r="L60" s="2">
+      <c r="L60" s="1">
         <v>1170</v>
       </c>
-      <c r="M60" s="2">
+      <c r="M60" s="1">
         <v>0.33</v>
       </c>
-      <c r="N60" s="2">
+      <c r="N60" s="1">
         <v>858</v>
       </c>
-      <c r="O60" s="2">
+      <c r="O60" s="1">
         <v>43.76</v>
       </c>
-      <c r="P60" s="2">
+      <c r="P60" s="1">
         <v>-116.1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+    <row r="61" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <v>7640</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="1">
         <v>5840</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61" s="1">
         <v>1800</v>
       </c>
-      <c r="F61" s="2">
+      <c r="F61" s="1">
         <v>5</v>
       </c>
-      <c r="G61" s="2">
+      <c r="G61" s="1">
         <v>46</v>
       </c>
-      <c r="H61" s="2">
+      <c r="H61" s="1">
         <v>1500</v>
       </c>
-      <c r="I61" s="2">
+      <c r="I61" s="1">
         <v>0.3</v>
       </c>
-      <c r="J61" s="2">
+      <c r="J61" s="1">
         <v>450</v>
       </c>
-      <c r="K61" s="2">
+      <c r="K61" s="1">
         <v>0.5</v>
       </c>
-      <c r="L61" s="2">
+      <c r="L61" s="1">
         <v>750</v>
       </c>
-      <c r="M61" s="2">
+      <c r="M61" s="1">
         <v>0.2</v>
       </c>
-      <c r="N61" s="2">
+      <c r="N61" s="1">
         <v>300</v>
       </c>
-      <c r="O61" s="2">
+      <c r="O61" s="1">
         <v>45.05</v>
       </c>
-      <c r="P61" s="2">
+      <c r="P61" s="1">
         <v>-116.12</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+    <row r="62" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <v>5565</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="1">
         <v>4280</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62" s="1">
         <v>845</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="1">
         <v>2</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62" s="1">
         <v>7</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62" s="1">
         <v>260</v>
       </c>
-      <c r="I62" s="2">
+      <c r="I62" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J62" s="2">
+      <c r="J62" s="1">
         <v>72.8</v>
       </c>
-      <c r="K62" s="2">
+      <c r="K62" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L62" s="2">
+      <c r="L62" s="1">
         <v>75.400000000000006</v>
       </c>
-      <c r="M62" s="2">
+      <c r="M62" s="1">
         <v>0.43</v>
       </c>
-      <c r="N62" s="2">
+      <c r="N62" s="1">
         <v>111.8</v>
       </c>
-      <c r="O62" s="2">
+      <c r="O62" s="1">
         <v>46.06</v>
       </c>
-      <c r="P62" s="2">
+      <c r="P62" s="1">
         <v>-116.46</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+    <row r="63" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <v>6600</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="1">
         <v>5600</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="1">
         <v>1000</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63" s="1">
         <v>6</v>
       </c>
-      <c r="G63" s="2">
+      <c r="G63" s="1">
         <v>16</v>
       </c>
-      <c r="H63" s="2">
+      <c r="H63" s="1">
         <v>640</v>
       </c>
-      <c r="I63" s="2">
+      <c r="I63" s="1">
         <v>0.35</v>
       </c>
-      <c r="J63" s="2">
+      <c r="J63" s="1">
         <v>224</v>
       </c>
-      <c r="K63" s="2">
+      <c r="K63" s="1">
         <v>0.45</v>
       </c>
-      <c r="L63" s="2">
+      <c r="L63" s="1">
         <v>288</v>
       </c>
-      <c r="M63" s="2">
+      <c r="M63" s="1">
         <v>0.2</v>
       </c>
-      <c r="N63" s="2">
+      <c r="N63" s="1">
         <v>128</v>
       </c>
-      <c r="O63" s="2">
+      <c r="O63" s="1">
         <v>44.14</v>
       </c>
-      <c r="P63" s="2">
+      <c r="P63" s="1">
         <v>-112.7</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+    <row r="64" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="1">
         <v>5700</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64" s="1">
         <v>405</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="1">
         <v>1</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G64" s="1">
         <v>5</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H64" s="1">
         <v>40</v>
       </c>
-      <c r="I64" s="2">
+      <c r="I64" s="1">
         <v>0.35</v>
       </c>
-      <c r="J64" s="2">
+      <c r="J64" s="1">
         <v>14</v>
       </c>
-      <c r="K64" s="2">
+      <c r="K64" s="1">
         <v>0.45</v>
       </c>
-      <c r="L64" s="2">
+      <c r="L64" s="1">
         <v>18</v>
       </c>
-      <c r="M64" s="2">
+      <c r="M64" s="1">
         <v>0.2</v>
       </c>
-      <c r="N64" s="2">
+      <c r="N64" s="1">
         <v>8</v>
       </c>
-      <c r="O64" s="2">
+      <c r="O64" s="1">
         <v>44.93</v>
       </c>
-      <c r="P64" s="2">
+      <c r="P64" s="1">
         <v>-116.16</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="1">
         <v>5650</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="1">
         <v>4500</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65" s="1">
         <v>1150</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F65" s="1">
         <v>4</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G65" s="1">
         <v>34</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65" s="1">
         <v>540</v>
       </c>
-      <c r="I65" s="2">
+      <c r="I65" s="1">
         <v>0.2</v>
       </c>
-      <c r="J65" s="2">
+      <c r="J65" s="1">
         <v>108</v>
       </c>
-      <c r="K65" s="2">
+      <c r="K65" s="1">
         <v>0.5</v>
       </c>
-      <c r="L65" s="2">
+      <c r="L65" s="1">
         <v>270</v>
       </c>
-      <c r="M65" s="2">
+      <c r="M65" s="1">
         <v>0.3</v>
       </c>
-      <c r="N65" s="2">
+      <c r="N65" s="1">
         <v>162</v>
       </c>
-      <c r="O65" s="2">
+      <c r="O65" s="1">
         <v>47.47</v>
       </c>
-      <c r="P65" s="2">
+      <c r="P65" s="1">
         <v>-115.69</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
+    <row r="66" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="1">
         <v>7240</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="1">
         <v>6500</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66" s="1">
         <v>700</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F66" s="1">
         <v>3</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66" s="1">
         <v>11</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66" s="1">
         <v>120</v>
       </c>
-      <c r="I66" s="2">
+      <c r="I66" s="1">
         <v>0.3</v>
       </c>
-      <c r="J66" s="2">
+      <c r="J66" s="1">
         <v>36</v>
       </c>
-      <c r="K66" s="2">
+      <c r="K66" s="1">
         <v>0.25</v>
       </c>
-      <c r="L66" s="2">
+      <c r="L66" s="1">
         <v>30</v>
       </c>
-      <c r="M66" s="2">
+      <c r="M66" s="1">
         <v>0.45</v>
       </c>
-      <c r="N66" s="2">
+      <c r="N66" s="1">
         <v>54</v>
       </c>
-      <c r="O66" s="2">
+      <c r="O66" s="1">
         <v>42.2</v>
       </c>
-      <c r="P66" s="2">
+      <c r="P66" s="1">
         <v>-114.41</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+    <row r="67" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="1">
         <v>8560</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="1">
         <v>6300</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67" s="1">
         <v>2200</v>
       </c>
-      <c r="F67" s="2">
+      <c r="F67" s="1">
         <v>3</v>
       </c>
-      <c r="G67" s="2">
+      <c r="G67" s="1">
         <v>54</v>
       </c>
-      <c r="H67" s="2">
+      <c r="H67" s="1">
         <v>1100</v>
       </c>
-      <c r="I67" s="2">
+      <c r="I67" s="1">
         <v>0.12</v>
       </c>
-      <c r="J67" s="2">
+      <c r="J67" s="1">
         <v>132</v>
       </c>
-      <c r="K67" s="2">
+      <c r="K67" s="1">
         <v>0.35</v>
       </c>
-      <c r="L67" s="2">
+      <c r="L67" s="1">
         <v>385</v>
       </c>
-      <c r="M67" s="2">
+      <c r="M67" s="1">
         <v>0.53</v>
       </c>
-      <c r="N67" s="2">
+      <c r="N67" s="1">
         <v>583</v>
       </c>
-      <c r="O67" s="2">
+      <c r="O67" s="1">
         <v>42.74</v>
       </c>
-      <c r="P67" s="2">
+      <c r="P67" s="1">
         <v>-112.03</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+    <row r="68" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="1">
         <v>9000</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="1">
         <v>8000</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68" s="1">
         <v>1000</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68" s="1">
         <v>3</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G68" s="1">
         <v>24</v>
       </c>
-      <c r="H68" s="2">
+      <c r="H68" s="1">
         <v>500</v>
       </c>
-      <c r="I68" s="2">
+      <c r="I68" s="1">
         <v>0.35</v>
       </c>
-      <c r="J68" s="2">
+      <c r="J68" s="1">
         <v>175</v>
       </c>
-      <c r="K68" s="2">
+      <c r="K68" s="1">
         <v>0.4</v>
       </c>
-      <c r="L68" s="2">
+      <c r="L68" s="1">
         <v>200</v>
       </c>
-      <c r="M68" s="2">
+      <c r="M68" s="1">
         <v>0.25</v>
       </c>
-      <c r="N68" s="2">
+      <c r="N68" s="1">
         <v>125</v>
       </c>
-      <c r="O68" s="2">
+      <c r="O68" s="1">
         <v>42.32</v>
       </c>
-      <c r="P68" s="2">
+      <c r="P68" s="1">
         <v>-113.61</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+    <row r="69" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="1">
         <v>6400</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="1">
         <v>4000</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69" s="1">
         <v>2400</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F69" s="1">
         <v>9</v>
       </c>
-      <c r="G69" s="2">
+      <c r="G69" s="1">
         <v>92</v>
       </c>
-      <c r="H69" s="2">
+      <c r="H69" s="1">
         <v>2900</v>
       </c>
-      <c r="I69" s="2">
+      <c r="I69" s="1">
         <v>0.1</v>
       </c>
-      <c r="J69" s="2">
+      <c r="J69" s="1">
         <v>290</v>
       </c>
-      <c r="K69" s="2">
+      <c r="K69" s="1">
         <v>0.4</v>
       </c>
-      <c r="L69" s="2">
+      <c r="L69" s="1">
         <v>1160</v>
       </c>
-      <c r="M69" s="2">
+      <c r="M69" s="1">
         <v>0.5</v>
       </c>
-      <c r="N69" s="2">
+      <c r="N69" s="1">
         <v>1450</v>
       </c>
-      <c r="O69" s="2">
+      <c r="O69" s="1">
         <v>48.35</v>
       </c>
-      <c r="P69" s="2">
+      <c r="P69" s="1">
         <v>-116.59</v>
       </c>
     </row>

</xml_diff>